<commit_message>
feat: Added scenario selection
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7AA1BF6-8620-4AA8-903F-892A0AE97A98}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA130069-B53A-432E-8D0D-8183C1BFB86E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
@@ -105,12 +105,6 @@
     <t>UN</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>N20 Present</t>
-  </si>
-  <si>
     <t>Production (tonnes/year)</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Number of Years</t>
+  </si>
+  <si>
+    <t>N2O Present</t>
   </si>
 </sst>
 </file>
@@ -630,10 +630,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -954,8 +950,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,33 +963,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>100000</v>
@@ -1015,7 +1011,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: Added Discounts to Volume data.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9143B857-80F6-40AD-B8CD-511B1D6C69F9}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D60EB47A-9B0B-4F7A-BA37-D463050DB8A8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
     <sheet name="Fertilizer Displacement Table" sheetId="3" r:id="rId3"/>
+    <sheet name="Discounts to Volume Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="55">
   <si>
     <t>Case Number</t>
   </si>
@@ -162,6 +163,48 @@
   <si>
     <t>Ratio to UAN</t>
   </si>
+  <si>
+    <t>Waste Diversion</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Landfill</t>
+  </si>
+  <si>
+    <t>regulatory additionality</t>
+  </si>
+  <si>
+    <t>Stockpile</t>
+  </si>
+  <si>
+    <t>Incineration</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>Compost</t>
+  </si>
+  <si>
+    <t>Land Use</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Leakage</t>
+  </si>
+  <si>
+    <t>N2O</t>
+  </si>
 </sst>
 </file>
 
@@ -250,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -542,6 +585,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -549,7 +623,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -640,6 +714,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1054,7 +1151,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7029,7 +7126,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -7213,4 +7310,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46A4060-5135-400D-B9B9-8A57ADBEE3EA}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="51">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="54">
+        <v>0</v>
+      </c>
+      <c r="D3" s="55">
+        <v>0</v>
+      </c>
+      <c r="E3" s="52"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="54">
+        <v>0</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0</v>
+      </c>
+      <c r="E4" s="52"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="54">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="54">
+        <v>0</v>
+      </c>
+      <c r="D7" s="55">
+        <v>0</v>
+      </c>
+      <c r="E7" s="52"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Added Pricing Table.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D60EB47A-9B0B-4F7A-BA37-D463050DB8A8}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B4C2005-4D5A-4119-8CD2-1F4CD01F0F55}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Fertilizer Displacement Table" sheetId="3" r:id="rId3"/>
-    <sheet name="Discounts to Volume Table" sheetId="4" r:id="rId4"/>
+    <sheet name="Pricing Table" sheetId="5" r:id="rId3"/>
+    <sheet name="Fertilizer Displacement Table" sheetId="3" r:id="rId4"/>
+    <sheet name="Discounts to Volume Table" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="63">
   <si>
     <t>Case Number</t>
   </si>
@@ -205,15 +206,41 @@
   <si>
     <t>N2O</t>
   </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>N2O (industrial)</t>
+  </si>
+  <si>
+    <t>Gold Average</t>
+  </si>
+  <si>
+    <t>Verra Average</t>
+  </si>
+  <si>
+    <t>Offset Discount</t>
+  </si>
+  <si>
+    <t>Transaction Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Volume</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -617,13 +644,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -673,12 +701,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -699,21 +721,6 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,9 +744,38 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
@@ -1087,16 +1123,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="35" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="35"/>
-    <col min="4" max="4" width="13.140625" style="35" customWidth="1"/>
-    <col min="5" max="5" width="15" style="35" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="35"/>
-    <col min="7" max="7" width="15.42578125" style="35" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="29" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="29"/>
+    <col min="4" max="4" width="13.140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="15" style="29" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="29"/>
+    <col min="7" max="7" width="15.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1114,30 +1150,30 @@
       <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="35">
-        <v>10</v>
-      </c>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="29">
+        <v>10</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="29">
         <v>100000</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="30">
         <v>0.5</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="31">
         <v>0.1</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="32">
         <v>25</v>
       </c>
     </row>
@@ -1151,7 +1187,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1168,7 +1204,7 @@
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="32" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,13 +1214,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -7122,189 +7158,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F222E5FA-6EF1-439E-B4E5-C313891F9DB1}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E95648-8BEC-4E9E-BC95-5FC06BCB4F47}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="43" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
-        <v>0.19949999999999998</v>
-      </c>
-      <c r="B2" s="23">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23">
-        <v>0</v>
-      </c>
-      <c r="D2" s="23">
-        <v>0.22799999999999998</v>
-      </c>
-      <c r="E2" s="23">
-        <v>0.05</v>
-      </c>
-      <c r="F2" s="24">
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="G2" s="24">
-        <v>1.8136363636363633</v>
-      </c>
-      <c r="H2" s="24">
-        <v>1.1083333333333332</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0.58676470588235285</v>
-      </c>
-      <c r="J2" s="24">
-        <v>0.43369565217391298</v>
-      </c>
-      <c r="K2" s="25">
-        <v>0.62343749999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
-        <v>0.189</v>
-      </c>
-      <c r="B3" s="23">
-        <v>0</v>
-      </c>
-      <c r="C3" s="23">
-        <v>0</v>
-      </c>
-      <c r="D3" s="23">
-        <v>0.216</v>
-      </c>
-      <c r="E3" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="24">
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="G3" s="24">
-        <v>1.7181818181818183</v>
-      </c>
-      <c r="H3" s="24">
-        <v>1.05</v>
-      </c>
-      <c r="I3" s="24">
-        <v>0.55588235294117638</v>
-      </c>
-      <c r="J3" s="24">
-        <v>0.41086956521739126</v>
-      </c>
-      <c r="K3" s="25">
-        <v>0.59062499999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
-        <v>0.17849999999999999</v>
-      </c>
-      <c r="B4" s="23">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23">
-        <v>0</v>
-      </c>
-      <c r="D4" s="23">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="E4" s="23">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.85</v>
-      </c>
-      <c r="G4" s="24">
-        <v>1.6227272727272726</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.9916666666666667</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="J4" s="24">
-        <v>0.38804347826086955</v>
-      </c>
-      <c r="K4" s="25">
-        <v>0.55781249999999993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="B5" s="26">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26">
-        <v>0</v>
-      </c>
-      <c r="D5" s="26">
-        <v>0.192</v>
-      </c>
-      <c r="E5" s="26">
+    <row r="1" spans="1:9" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="62">
+        <v>2.5</v>
+      </c>
+      <c r="B2" s="63">
+        <v>4.37</v>
+      </c>
+      <c r="C2" s="63">
+        <v>1.9</v>
+      </c>
+      <c r="D2" s="64">
+        <v>282300000</v>
+      </c>
+      <c r="E2" s="65">
+        <v>100400000</v>
+      </c>
+      <c r="F2" s="63">
+        <v>5.27</v>
+      </c>
+      <c r="G2" s="63">
+        <v>3.84</v>
+      </c>
+      <c r="H2" s="66">
         <v>0.2</v>
       </c>
-      <c r="F5" s="27">
-        <v>0.80000000000000016</v>
-      </c>
-      <c r="G5" s="27">
-        <v>1.5272727272727273</v>
-      </c>
-      <c r="H5" s="27">
-        <v>0.93333333333333335</v>
-      </c>
-      <c r="I5" s="27">
-        <v>0.49411764705882355</v>
-      </c>
-      <c r="J5" s="27">
-        <v>0.36521739130434783</v>
-      </c>
-      <c r="K5" s="28">
-        <v>0.52500000000000002</v>
+      <c r="I2" s="67">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7313,164 +7240,359 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F222E5FA-6EF1-439E-B4E5-C313891F9DB1}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="53" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="54">
+        <v>0.19949999999999998</v>
+      </c>
+      <c r="B2" s="54">
+        <v>0</v>
+      </c>
+      <c r="C2" s="54">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54">
+        <v>0.22799999999999998</v>
+      </c>
+      <c r="E2" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="55">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="G2" s="55">
+        <v>1.8136363636363633</v>
+      </c>
+      <c r="H2" s="55">
+        <v>1.1083333333333332</v>
+      </c>
+      <c r="I2" s="55">
+        <v>0.58676470588235285</v>
+      </c>
+      <c r="J2" s="55">
+        <v>0.43369565217391298</v>
+      </c>
+      <c r="K2" s="56">
+        <v>0.62343749999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="54">
+        <v>0.189</v>
+      </c>
+      <c r="B3" s="54">
+        <v>0</v>
+      </c>
+      <c r="C3" s="54">
+        <v>0</v>
+      </c>
+      <c r="D3" s="54">
+        <v>0.216</v>
+      </c>
+      <c r="E3" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="55">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="G3" s="55">
+        <v>1.7181818181818183</v>
+      </c>
+      <c r="H3" s="55">
+        <v>1.05</v>
+      </c>
+      <c r="I3" s="55">
+        <v>0.55588235294117638</v>
+      </c>
+      <c r="J3" s="55">
+        <v>0.41086956521739126</v>
+      </c>
+      <c r="K3" s="56">
+        <v>0.59062499999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="54">
+        <v>0.17849999999999999</v>
+      </c>
+      <c r="B4" s="54">
+        <v>0</v>
+      </c>
+      <c r="C4" s="54">
+        <v>0</v>
+      </c>
+      <c r="D4" s="54">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E4" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="55">
+        <v>0.85</v>
+      </c>
+      <c r="G4" s="55">
+        <v>1.6227272727272726</v>
+      </c>
+      <c r="H4" s="55">
+        <v>0.9916666666666667</v>
+      </c>
+      <c r="I4" s="55">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="J4" s="55">
+        <v>0.38804347826086955</v>
+      </c>
+      <c r="K4" s="56">
+        <v>0.55781249999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="B5" s="57">
+        <v>0</v>
+      </c>
+      <c r="C5" s="57">
+        <v>0</v>
+      </c>
+      <c r="D5" s="57">
+        <v>0.192</v>
+      </c>
+      <c r="E5" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="58">
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="G5" s="58">
+        <v>1.5272727272727273</v>
+      </c>
+      <c r="H5" s="58">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="I5" s="58">
+        <v>0.49411764705882355</v>
+      </c>
+      <c r="J5" s="58">
+        <v>0.36521739130434783</v>
+      </c>
+      <c r="K5" s="59">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46A4060-5135-400D-B9B9-8A57ADBEE3EA}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="50">
+      <c r="C2" s="39">
         <v>0.8</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="40">
         <v>0.6</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="54">
-        <v>0</v>
-      </c>
-      <c r="D3" s="55">
-        <v>0</v>
-      </c>
-      <c r="E3" s="52"/>
+      <c r="C3" s="43">
+        <v>0</v>
+      </c>
+      <c r="D3" s="44">
+        <v>0</v>
+      </c>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="54">
-        <v>0</v>
-      </c>
-      <c r="D4" s="55">
-        <v>0</v>
-      </c>
-      <c r="E4" s="52"/>
+      <c r="C4" s="43">
+        <v>0</v>
+      </c>
+      <c r="D4" s="44">
+        <v>0</v>
+      </c>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="43">
         <v>0.8</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="44">
         <v>0.6</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="52" t="s">
+      <c r="A6" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="43">
         <v>0.2</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="44">
         <v>0.2</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="54">
-        <v>0</v>
-      </c>
-      <c r="D7" s="55">
-        <v>0</v>
-      </c>
-      <c r="E7" s="52"/>
+      <c r="C7" s="43">
+        <v>0</v>
+      </c>
+      <c r="D7" s="44">
+        <v>0</v>
+      </c>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="39">
         <v>0.5</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="40">
         <v>0.2</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="38" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="48">
         <v>0.5</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="49">
         <v>0.2</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="47" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Added Fertilizer Displacement Calculations
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B4C2005-4D5A-4119-8CD2-1F4CD01F0F55}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED15D765-BC11-41F1-87BF-A13487AF515D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
     <sheet name="Pricing Table" sheetId="5" r:id="rId3"/>
-    <sheet name="Fertilizer Displacement Table" sheetId="3" r:id="rId4"/>
+    <sheet name="Nutriant Table" sheetId="3" r:id="rId4"/>
     <sheet name="Discounts to Volume Table" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="59">
   <si>
     <t>Case Number</t>
   </si>
@@ -147,24 +147,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Ratio to AS</t>
-  </si>
-  <si>
-    <t>Ratio to MAP</t>
-  </si>
-  <si>
-    <t>Ratio to DAP</t>
-  </si>
-  <si>
-    <t>Ratio to AN</t>
-  </si>
-  <si>
-    <t>Ratio to Urea</t>
-  </si>
-  <si>
-    <t>Ratio to UAN</t>
-  </si>
-  <si>
     <t>Waste Diversion</t>
   </si>
   <si>
@@ -229,6 +211,12 @@
   </si>
   <si>
     <t>Total Volume</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>DAP</t>
   </si>
 </sst>
 </file>
@@ -651,7 +639,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -744,9 +732,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -757,7 +742,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -772,6 +756,12 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7159,9 +7149,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E95648-8BEC-4E9E-BC95-5FC06BCB4F47}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7176,61 +7167,61 @@
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="60" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="58" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="E1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>57</v>
-      </c>
       <c r="G1" s="34" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="61" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="I1" s="59" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62">
+      <c r="A2" s="60">
         <v>2.5</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="61">
         <v>4.37</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="61">
         <v>1.9</v>
       </c>
-      <c r="D2" s="64">
+      <c r="D2" s="62">
         <v>282300000</v>
       </c>
-      <c r="E2" s="65">
+      <c r="E2" s="63">
         <v>100400000</v>
       </c>
-      <c r="F2" s="63">
+      <c r="F2" s="61">
         <v>5.27</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="61">
         <v>3.84</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="64">
         <v>0.2</v>
       </c>
-      <c r="I2" s="67">
+      <c r="I2" s="65">
         <v>1</v>
       </c>
     </row>
@@ -7242,189 +7233,203 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F222E5FA-6EF1-439E-B4E5-C313891F9DB1}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="17.28515625" style="29" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="53" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:12" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="54">
+      <c r="G1" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="67">
+        <v>5</v>
+      </c>
+      <c r="B2" s="53">
         <v>0.19949999999999998</v>
       </c>
-      <c r="B2" s="54">
-        <v>0</v>
-      </c>
-      <c r="C2" s="54">
-        <v>0</v>
-      </c>
-      <c r="D2" s="54">
+      <c r="C2" s="53">
+        <v>0</v>
+      </c>
+      <c r="D2" s="53">
+        <v>0</v>
+      </c>
+      <c r="E2" s="53">
         <v>0.22799999999999998</v>
       </c>
-      <c r="E2" s="54">
+      <c r="F2" s="53">
         <v>0.05</v>
       </c>
-      <c r="F2" s="55">
+      <c r="G2" s="66">
         <v>0.95000000000000007</v>
       </c>
-      <c r="G2" s="55">
+      <c r="H2" s="66">
         <v>1.8136363636363633</v>
       </c>
-      <c r="H2" s="55">
+      <c r="I2" s="66">
         <v>1.1083333333333332</v>
       </c>
-      <c r="I2" s="55">
+      <c r="J2" s="66">
         <v>0.58676470588235285</v>
       </c>
-      <c r="J2" s="55">
+      <c r="K2" s="66">
         <v>0.43369565217391298</v>
       </c>
-      <c r="K2" s="56">
+      <c r="L2" s="54">
         <v>0.62343749999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="67">
+        <v>10</v>
+      </c>
+      <c r="B3" s="53">
         <v>0.189</v>
       </c>
-      <c r="B3" s="54">
-        <v>0</v>
-      </c>
-      <c r="C3" s="54">
-        <v>0</v>
-      </c>
-      <c r="D3" s="54">
+      <c r="C3" s="53">
+        <v>0</v>
+      </c>
+      <c r="D3" s="53">
+        <v>0</v>
+      </c>
+      <c r="E3" s="53">
         <v>0.216</v>
       </c>
-      <c r="E3" s="54">
+      <c r="F3" s="53">
         <v>0.1</v>
       </c>
-      <c r="F3" s="55">
+      <c r="G3" s="66">
         <v>0.89999999999999991</v>
       </c>
-      <c r="G3" s="55">
+      <c r="H3" s="66">
         <v>1.7181818181818183</v>
       </c>
-      <c r="H3" s="55">
+      <c r="I3" s="66">
         <v>1.05</v>
       </c>
-      <c r="I3" s="55">
+      <c r="J3" s="66">
         <v>0.55588235294117638</v>
       </c>
-      <c r="J3" s="55">
+      <c r="K3" s="66">
         <v>0.41086956521739126</v>
       </c>
-      <c r="K3" s="56">
+      <c r="L3" s="54">
         <v>0.59062499999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="54">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="67">
+        <v>15</v>
+      </c>
+      <c r="B4" s="53">
         <v>0.17849999999999999</v>
       </c>
-      <c r="B4" s="54">
-        <v>0</v>
-      </c>
-      <c r="C4" s="54">
-        <v>0</v>
-      </c>
-      <c r="D4" s="54">
+      <c r="C4" s="53">
+        <v>0</v>
+      </c>
+      <c r="D4" s="53">
+        <v>0</v>
+      </c>
+      <c r="E4" s="53">
         <v>0.20399999999999999</v>
       </c>
-      <c r="E4" s="54">
+      <c r="F4" s="53">
         <v>0.15</v>
       </c>
-      <c r="F4" s="55">
+      <c r="G4" s="66">
         <v>0.85</v>
       </c>
-      <c r="G4" s="55">
+      <c r="H4" s="66">
         <v>1.6227272727272726</v>
       </c>
-      <c r="H4" s="55">
+      <c r="I4" s="66">
         <v>0.9916666666666667</v>
       </c>
-      <c r="I4" s="55">
+      <c r="J4" s="66">
         <v>0.52500000000000002</v>
       </c>
-      <c r="J4" s="55">
+      <c r="K4" s="66">
         <v>0.38804347826086955</v>
       </c>
-      <c r="K4" s="56">
+      <c r="L4" s="54">
         <v>0.55781249999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57">
+    <row r="5" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="68">
+        <v>20</v>
+      </c>
+      <c r="B5" s="55">
         <v>0.16800000000000001</v>
       </c>
-      <c r="B5" s="57">
-        <v>0</v>
-      </c>
-      <c r="C5" s="57">
-        <v>0</v>
-      </c>
-      <c r="D5" s="57">
+      <c r="C5" s="55">
+        <v>0</v>
+      </c>
+      <c r="D5" s="55">
+        <v>0</v>
+      </c>
+      <c r="E5" s="55">
         <v>0.192</v>
       </c>
-      <c r="E5" s="57">
+      <c r="F5" s="55">
         <v>0.2</v>
       </c>
-      <c r="F5" s="58">
+      <c r="G5" s="56">
         <v>0.80000000000000016</v>
       </c>
-      <c r="G5" s="58">
+      <c r="H5" s="56">
         <v>1.5272727272727273</v>
       </c>
-      <c r="H5" s="58">
+      <c r="I5" s="56">
         <v>0.93333333333333335</v>
       </c>
-      <c r="I5" s="58">
+      <c r="J5" s="56">
         <v>0.49411764705882355</v>
       </c>
-      <c r="J5" s="58">
+      <c r="K5" s="56">
         <v>0.36521739130434783</v>
       </c>
-      <c r="K5" s="59">
+      <c r="L5" s="57">
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -7451,10 +7456,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>12</v>
@@ -7463,15 +7468,15 @@
         <v>13</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" s="39">
         <v>0.8</v>
@@ -7480,15 +7485,15 @@
         <v>0.6</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C3" s="43">
         <v>0</v>
@@ -7500,10 +7505,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C4" s="43">
         <v>0</v>
@@ -7515,10 +7520,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="43">
         <v>0.8</v>
@@ -7527,7 +7532,7 @@
         <v>0.6</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -7535,7 +7540,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C6" s="43">
         <v>0.2</v>
@@ -7544,7 +7549,7 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7552,7 +7557,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" s="43">
         <v>0</v>
@@ -7564,10 +7569,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C8" s="39">
         <v>0.5</v>
@@ -7576,15 +7581,15 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="48">
         <v>0.5</v>
@@ -7593,7 +7598,7 @@
         <v>0.2</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added Adjusted Standard Volumes Discount fields.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F07028-EF57-413C-A6D9-D0ACAB48837A}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BEDC07B-FB54-424E-BF75-6E8C2C570D16}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="57">
   <si>
     <t>Product Made</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Incineration</t>
-  </si>
-  <si>
-    <t>AG</t>
   </si>
   <si>
     <t>Compost</t>
@@ -1171,7 +1168,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -6392,31 +6389,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="D1" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="58" t="s">
         <v>52</v>
-      </c>
-      <c r="I1" s="58" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6489,10 +6486,10 @@
         <v>10</v>
       </c>
       <c r="H1" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="49" t="s">
         <v>56</v>
-      </c>
-      <c r="I1" s="49" t="s">
-        <v>57</v>
       </c>
       <c r="J1" s="49" t="s">
         <v>17</v>
@@ -6666,8 +6663,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6743,7 +6740,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>38</v>
@@ -6763,7 +6760,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="42">
         <v>0.2</v>
@@ -6792,10 +6789,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>45</v>
       </c>
       <c r="C8" s="38">
         <v>0.5</v>
@@ -6804,15 +6801,15 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="47">
         <v>0.5</v>
@@ -6821,7 +6818,7 @@
         <v>0.2</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added market and standard price calculation function.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BEDC07B-FB54-424E-BF75-6E8C2C570D16}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5167FAB-55E9-4E5A-9270-9CA341858157}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>N2O Present</t>
   </si>
   <si>
-    <t>Emissions Permit Price</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>DAP</t>
+  </si>
+  <si>
+    <t>Emissions Permit Price</t>
   </si>
 </sst>
 </file>
@@ -697,9 +697,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -738,19 +735,22 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="25" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,7 +1099,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1132,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,13 +1148,13 @@
       <c r="D2" s="28">
         <v>100000</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="59">
         <v>0.5</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="60">
         <v>0.1</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="61">
         <v>25</v>
       </c>
     </row>
@@ -6372,8 +6372,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6387,61 +6387,61 @@
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:9" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="D1" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="58" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59">
+      <c r="A2" s="62">
         <v>2.5</v>
       </c>
-      <c r="B2" s="60">
+      <c r="B2" s="63">
         <v>4.37</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="63">
         <v>1.9</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="64">
         <v>282300000</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="65">
         <v>100400000</v>
       </c>
-      <c r="F2" s="60">
+      <c r="F2" s="63">
         <v>5.27</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="63">
         <v>3.84</v>
       </c>
-      <c r="H2" s="63">
+      <c r="H2" s="66">
         <v>0.2</v>
       </c>
-      <c r="I2" s="64">
+      <c r="I2" s="67">
         <v>1</v>
       </c>
     </row>
@@ -6455,7 +6455,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6463,193 +6465,193 @@
     <col min="2" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="51" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:12" s="48" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="47" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="66">
+      <c r="A2" s="56">
         <v>5</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="49">
         <v>0.19949999999999998</v>
       </c>
-      <c r="C2" s="52">
-        <v>0</v>
-      </c>
-      <c r="D2" s="52">
-        <v>0</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="C2" s="49">
+        <v>0</v>
+      </c>
+      <c r="D2" s="49">
+        <v>0</v>
+      </c>
+      <c r="E2" s="49">
         <v>0.22799999999999998</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="49">
         <v>0.05</v>
       </c>
-      <c r="G2" s="65">
+      <c r="G2" s="55">
         <v>0.95000000000000007</v>
       </c>
-      <c r="H2" s="65">
+      <c r="H2" s="55">
         <v>1.8136363636363633</v>
       </c>
-      <c r="I2" s="65">
+      <c r="I2" s="55">
         <v>1.1083333333333332</v>
       </c>
-      <c r="J2" s="65">
+      <c r="J2" s="55">
         <v>0.58676470588235285</v>
       </c>
-      <c r="K2" s="65">
+      <c r="K2" s="55">
         <v>0.43369565217391298</v>
       </c>
-      <c r="L2" s="53">
+      <c r="L2" s="50">
         <v>0.62343749999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="66">
-        <v>10</v>
-      </c>
-      <c r="B3" s="52">
+      <c r="A3" s="28">
+        <v>10</v>
+      </c>
+      <c r="B3" s="49">
         <v>0.189</v>
       </c>
-      <c r="C3" s="52">
-        <v>0</v>
-      </c>
-      <c r="D3" s="52">
-        <v>0</v>
-      </c>
-      <c r="E3" s="52">
+      <c r="C3" s="49">
+        <v>0</v>
+      </c>
+      <c r="D3" s="49">
+        <v>0</v>
+      </c>
+      <c r="E3" s="49">
         <v>0.216</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="49">
         <v>0.1</v>
       </c>
-      <c r="G3" s="65">
+      <c r="G3" s="55">
         <v>0.89999999999999991</v>
       </c>
-      <c r="H3" s="65">
+      <c r="H3" s="55">
         <v>1.7181818181818183</v>
       </c>
-      <c r="I3" s="65">
+      <c r="I3" s="55">
         <v>1.05</v>
       </c>
-      <c r="J3" s="65">
+      <c r="J3" s="55">
         <v>0.55588235294117638</v>
       </c>
-      <c r="K3" s="65">
+      <c r="K3" s="55">
         <v>0.41086956521739126</v>
       </c>
-      <c r="L3" s="53">
+      <c r="L3" s="50">
         <v>0.59062499999999996</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="66">
-        <v>15</v>
-      </c>
-      <c r="B4" s="52">
+      <c r="A4" s="28">
+        <v>15</v>
+      </c>
+      <c r="B4" s="49">
         <v>0.17849999999999999</v>
       </c>
-      <c r="C4" s="52">
-        <v>0</v>
-      </c>
-      <c r="D4" s="52">
-        <v>0</v>
-      </c>
-      <c r="E4" s="52">
+      <c r="C4" s="49">
+        <v>0</v>
+      </c>
+      <c r="D4" s="49">
+        <v>0</v>
+      </c>
+      <c r="E4" s="49">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="49">
         <v>0.15</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="55">
         <v>0.85</v>
       </c>
-      <c r="H4" s="65">
+      <c r="H4" s="55">
         <v>1.6227272727272726</v>
       </c>
-      <c r="I4" s="65">
+      <c r="I4" s="55">
         <v>0.9916666666666667</v>
       </c>
-      <c r="J4" s="65">
+      <c r="J4" s="55">
         <v>0.52500000000000002</v>
       </c>
-      <c r="K4" s="65">
+      <c r="K4" s="55">
         <v>0.38804347826086955</v>
       </c>
-      <c r="L4" s="53">
+      <c r="L4" s="50">
         <v>0.55781249999999993</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67">
+      <c r="A5" s="57">
         <v>20</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="51">
         <v>0.16800000000000001</v>
       </c>
-      <c r="C5" s="54">
-        <v>0</v>
-      </c>
-      <c r="D5" s="54">
-        <v>0</v>
-      </c>
-      <c r="E5" s="54">
+      <c r="C5" s="51">
+        <v>0</v>
+      </c>
+      <c r="D5" s="51">
+        <v>0</v>
+      </c>
+      <c r="E5" s="51">
         <v>0.192</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="51">
         <v>0.2</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="52">
         <v>0.80000000000000016</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="52">
         <v>1.5272727272727273</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="52">
         <v>0.93333333333333335</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="52">
         <v>0.49411764705882355</v>
       </c>
-      <c r="K5" s="55">
+      <c r="K5" s="52">
         <v>0.36521739130434783</v>
       </c>
-      <c r="L5" s="56">
+      <c r="L5" s="53">
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -6663,7 +6665,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -6675,150 +6677,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="C1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="35" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="C2" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="38">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="39">
+        <v>0</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0</v>
+      </c>
+      <c r="E3" s="37"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0</v>
+      </c>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="39">
         <v>0.8</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D5" s="40">
         <v>0.6</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="E5" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="42">
-        <v>0</v>
-      </c>
-      <c r="D3" s="43">
-        <v>0</v>
-      </c>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="42">
-        <v>0</v>
-      </c>
-      <c r="D4" s="43">
-        <v>0</v>
-      </c>
-      <c r="E4" s="40"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="D5" s="43">
-        <v>0.6</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="40" t="s">
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0</v>
+      </c>
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="42">
+      <c r="B8" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="36">
         <v>0.2</v>
       </c>
-      <c r="D6" s="43">
+      <c r="E8" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="45">
         <v>0.2</v>
       </c>
-      <c r="E6" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="42">
-        <v>0</v>
-      </c>
-      <c r="D7" s="43">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="37" t="s">
+      <c r="E9" s="43" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="48">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added scenario calculation/output for multiple years.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5167FAB-55E9-4E5A-9270-9CA341858157}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C1D312-75E4-4216-92A5-DC5C5A680239}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="55">
   <si>
     <t>Product Made</t>
   </si>
@@ -108,19 +108,10 @@
     <t>Fee Allowance Portion</t>
   </si>
   <si>
-    <t>Scenario Name</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>NPV</t>
-  </si>
-  <si>
-    <t>Test Scenario</t>
-  </si>
-  <si>
-    <t>Number of Years</t>
   </si>
   <si>
     <t>N2O Present</t>
@@ -212,13 +203,15 @@
   <si>
     <t>Emissions Permit Price</t>
   </si>
+  <si>
+    <t>No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -633,7 +626,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -690,12 +683,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -742,8 +729,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="25" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -753,6 +738,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -761,7 +750,146 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -776,6 +904,20 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3922DC48-902B-40FA-9101-DF2CD964F26E}" name="Table3" displayName="Table3" ref="A1:E11" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E11" xr:uid="{3922DC48-902B-40FA-9101-DF2CD964F26E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{72AD1251-FFEE-4F0B-9CB0-3636EA240B75}" name="N2O Present" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{057619A2-247D-41E6-8773-AB7650AE734A}" name="Production (tonnes/year)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{6105223C-BC4F-4B7B-9DBA-CE2AD01000F3}" name="Fee Allowance Portion" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{32B80B58-EBA0-43FF-8303-1C48E9064AE6}" name="NPV" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{061B8E57-0E70-4336-9E84-F7639F3AE69F}" name="Emissions Permit Price" dataDxfId="0" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1096,70 +1238,213 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AFB15E-BA71-4499-B2BD-1FB153E20E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="28" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="28"/>
-    <col min="4" max="4" width="13.140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="15" style="28" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="28"/>
-    <col min="7" max="7" width="15.42578125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="16" style="26" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="14" style="26" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="26">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="65">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="26">
+        <v>125000</v>
+      </c>
+      <c r="C3" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="65">
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="26">
+        <v>135000</v>
+      </c>
+      <c r="C4" s="57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="65">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="26">
+        <v>145000</v>
+      </c>
+      <c r="C5" s="57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D5" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="65">
+        <v>25.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="26">
+        <v>150000</v>
+      </c>
+      <c r="C6" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="65">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="26">
+        <v>145000</v>
+      </c>
+      <c r="C7" s="57">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="65">
+        <v>25.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="26">
+        <v>135000</v>
+      </c>
+      <c r="C8" s="57">
+        <v>0.45</v>
+      </c>
+      <c r="D8" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="65">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="28">
-        <v>10</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="28">
-        <v>100000</v>
-      </c>
-      <c r="E2" s="59">
-        <v>0.5</v>
-      </c>
-      <c r="F2" s="60">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="26">
+        <v>115000</v>
+      </c>
+      <c r="C9" s="57">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="57">
         <v>0.1</v>
       </c>
-      <c r="G2" s="61">
-        <v>25</v>
+      <c r="E9" s="65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="26">
+        <v>95000</v>
+      </c>
+      <c r="C10" s="57">
+        <v>0.35</v>
+      </c>
+      <c r="D10" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="26">
+        <v>75000</v>
+      </c>
+      <c r="C11" s="57">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="65">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6372,7 +6657,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -6387,61 +6672,61 @@
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="30" t="s">
+      <c r="H1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="30" t="s">
+      <c r="I1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="68" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62">
+      <c r="A2" s="58">
         <v>2.5</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="59">
         <v>4.37</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="59">
         <v>1.9</v>
       </c>
-      <c r="D2" s="64">
+      <c r="D2" s="60">
         <v>282300000</v>
       </c>
-      <c r="E2" s="65">
+      <c r="E2" s="61">
         <v>100400000</v>
       </c>
-      <c r="F2" s="63">
+      <c r="F2" s="59">
         <v>5.27</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="59">
         <v>3.84</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="62">
         <v>0.2</v>
       </c>
-      <c r="I2" s="67">
+      <c r="I2" s="63">
         <v>1</v>
       </c>
     </row>
@@ -6461,197 +6746,197 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="28" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="17.28515625" style="26" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="48" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
+    <row r="1" spans="1:12" s="46" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="F1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="46" t="s">
+      <c r="G1" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="56">
+      <c r="A2" s="54">
         <v>5</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="47">
         <v>0.19949999999999998</v>
       </c>
-      <c r="C2" s="49">
-        <v>0</v>
-      </c>
-      <c r="D2" s="49">
-        <v>0</v>
-      </c>
-      <c r="E2" s="49">
+      <c r="C2" s="47">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47">
+        <v>0</v>
+      </c>
+      <c r="E2" s="47">
         <v>0.22799999999999998</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="47">
         <v>0.05</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="53">
         <v>0.95000000000000007</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="53">
         <v>1.8136363636363633</v>
       </c>
-      <c r="I2" s="55">
+      <c r="I2" s="53">
         <v>1.1083333333333332</v>
       </c>
-      <c r="J2" s="55">
+      <c r="J2" s="53">
         <v>0.58676470588235285</v>
       </c>
-      <c r="K2" s="55">
+      <c r="K2" s="53">
         <v>0.43369565217391298</v>
       </c>
-      <c r="L2" s="50">
+      <c r="L2" s="48">
         <v>0.62343749999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
-        <v>10</v>
-      </c>
-      <c r="B3" s="49">
+      <c r="A3" s="26">
+        <v>10</v>
+      </c>
+      <c r="B3" s="47">
         <v>0.189</v>
       </c>
-      <c r="C3" s="49">
-        <v>0</v>
-      </c>
-      <c r="D3" s="49">
-        <v>0</v>
-      </c>
-      <c r="E3" s="49">
+      <c r="C3" s="47">
+        <v>0</v>
+      </c>
+      <c r="D3" s="47">
+        <v>0</v>
+      </c>
+      <c r="E3" s="47">
         <v>0.216</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="47">
         <v>0.1</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="53">
         <v>0.89999999999999991</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="53">
         <v>1.7181818181818183</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="53">
         <v>1.05</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="53">
         <v>0.55588235294117638</v>
       </c>
-      <c r="K3" s="55">
+      <c r="K3" s="53">
         <v>0.41086956521739126</v>
       </c>
-      <c r="L3" s="50">
+      <c r="L3" s="48">
         <v>0.59062499999999996</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
-        <v>15</v>
-      </c>
-      <c r="B4" s="49">
+      <c r="A4" s="26">
+        <v>15</v>
+      </c>
+      <c r="B4" s="47">
         <v>0.17849999999999999</v>
       </c>
-      <c r="C4" s="49">
-        <v>0</v>
-      </c>
-      <c r="D4" s="49">
-        <v>0</v>
-      </c>
-      <c r="E4" s="49">
+      <c r="C4" s="47">
+        <v>0</v>
+      </c>
+      <c r="D4" s="47">
+        <v>0</v>
+      </c>
+      <c r="E4" s="47">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F4" s="49">
+      <c r="F4" s="47">
         <v>0.15</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="53">
         <v>0.85</v>
       </c>
-      <c r="H4" s="55">
+      <c r="H4" s="53">
         <v>1.6227272727272726</v>
       </c>
-      <c r="I4" s="55">
+      <c r="I4" s="53">
         <v>0.9916666666666667</v>
       </c>
-      <c r="J4" s="55">
+      <c r="J4" s="53">
         <v>0.52500000000000002</v>
       </c>
-      <c r="K4" s="55">
+      <c r="K4" s="53">
         <v>0.38804347826086955</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="48">
         <v>0.55781249999999993</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57">
+      <c r="A5" s="55">
         <v>20</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="49">
         <v>0.16800000000000001</v>
       </c>
-      <c r="C5" s="51">
-        <v>0</v>
-      </c>
-      <c r="D5" s="51">
-        <v>0</v>
-      </c>
-      <c r="E5" s="51">
+      <c r="C5" s="49">
+        <v>0</v>
+      </c>
+      <c r="D5" s="49">
+        <v>0</v>
+      </c>
+      <c r="E5" s="49">
         <v>0.192</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="49">
         <v>0.2</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="50">
         <v>0.80000000000000016</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="50">
         <v>1.5272727272727273</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="50">
         <v>0.93333333333333335</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="50">
         <v>0.49411764705882355</v>
       </c>
-      <c r="K5" s="52">
+      <c r="K5" s="50">
         <v>0.36521739130434783</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="51">
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -6677,150 +6962,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="32" t="s">
+      <c r="C2" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C3" s="37">
+        <v>0</v>
+      </c>
+      <c r="D3" s="38">
+        <v>0</v>
+      </c>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C4" s="37">
+        <v>0</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0</v>
+      </c>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="37">
         <v>0.8</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D5" s="38">
         <v>0.6</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E5" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="37" t="s">
+      <c r="C6" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="39">
-        <v>0</v>
-      </c>
-      <c r="D3" s="40">
-        <v>0</v>
-      </c>
-      <c r="E3" s="37"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="37" t="s">
+      <c r="B8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="39">
-        <v>0</v>
-      </c>
-      <c r="D4" s="40">
-        <v>0</v>
-      </c>
-      <c r="E4" s="37"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="39">
-        <v>0.8</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0.6</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="37" t="s">
+      <c r="C8" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="39">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="43">
         <v>0.2</v>
       </c>
-      <c r="D6" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="39">
-        <v>0</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="36">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>44</v>
+      <c r="E9" s="41" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added docstrings and README.
</commit_message>
<xml_diff>
--- a/data/ag_data.xlsx
+++ b/data/ag_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee2fd0c31013e2b7/Desktop/Data/Scenario Analysis Agriculture GHG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C1D312-75E4-4216-92A5-DC5C5A680239}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="8_{315683C9-4771-4DBA-8040-FCE333394224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2C30F81-CEEB-4B49-A661-61CDAAF2F92F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{033F283C-2EC3-4E80-924F-E457BD1171A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Input" sheetId="2" r:id="rId1"/>
@@ -1240,7 +1240,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1453,8 +1453,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,11 +1512,11 @@
         <v>11</v>
       </c>
       <c r="F2" s="7">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G2" s="8">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H2" s="9">
         <v>0</v>
@@ -1539,11 +1539,11 @@
         <v>12</v>
       </c>
       <c r="F3" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G3" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H3" s="15">
         <v>0</v>
@@ -1566,10 +1566,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G4" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H4" s="15">
         <v>0</v>
@@ -1592,10 +1592,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G5" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H5" s="15">
         <v>0</v>
@@ -1618,11 +1618,11 @@
         <v>11</v>
       </c>
       <c r="F6" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G6" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H6" s="15">
         <v>0</v>
@@ -1645,11 +1645,11 @@
         <v>12</v>
       </c>
       <c r="F7" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G7" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H7" s="15">
         <v>0</v>
@@ -1672,10 +1672,10 @@
         <v>11</v>
       </c>
       <c r="F8" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G8" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H8" s="15">
         <v>0</v>
@@ -1698,10 +1698,10 @@
         <v>12</v>
       </c>
       <c r="F9" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G9" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H9" s="15">
         <v>0</v>
@@ -1724,10 +1724,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G10" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H10" s="15">
         <v>0</v>
@@ -1750,10 +1750,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G11" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H11" s="15">
         <v>0</v>
@@ -1776,10 +1776,10 @@
         <v>11</v>
       </c>
       <c r="F12" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G12" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H12" s="15">
         <v>0</v>
@@ -1802,10 +1802,10 @@
         <v>12</v>
       </c>
       <c r="F13" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G13" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H13" s="15">
         <v>0</v>
@@ -1828,11 +1828,11 @@
         <v>11</v>
       </c>
       <c r="F14" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G14" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H14" s="15">
         <v>0</v>
@@ -1855,11 +1855,11 @@
         <v>12</v>
       </c>
       <c r="F15" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G15" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H15" s="15">
         <v>0</v>
@@ -1882,10 +1882,10 @@
         <v>11</v>
       </c>
       <c r="F16" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G16" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H16" s="15">
         <v>0</v>
@@ -1908,10 +1908,10 @@
         <v>12</v>
       </c>
       <c r="F17" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G17" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H17" s="15">
         <v>0</v>
@@ -1934,11 +1934,11 @@
         <v>11</v>
       </c>
       <c r="F18" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G18" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H18" s="15">
         <v>0</v>
@@ -1961,11 +1961,11 @@
         <v>12</v>
       </c>
       <c r="F19" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G19" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H19" s="15">
         <v>0</v>
@@ -1988,10 +1988,10 @@
         <v>11</v>
       </c>
       <c r="F20" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G20" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H20" s="15">
         <v>0</v>
@@ -2014,10 +2014,10 @@
         <v>12</v>
       </c>
       <c r="F21" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G21" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H21" s="15">
         <v>0</v>
@@ -2040,10 +2040,10 @@
         <v>11</v>
       </c>
       <c r="F22" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G22" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H22" s="15">
         <v>0</v>
@@ -2066,10 +2066,10 @@
         <v>12</v>
       </c>
       <c r="F23" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G23" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H23" s="15">
         <v>0</v>
@@ -2092,10 +2092,10 @@
         <v>11</v>
       </c>
       <c r="F24" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G24" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H24" s="15">
         <v>0</v>
@@ -2118,10 +2118,10 @@
         <v>12</v>
       </c>
       <c r="F25" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G25" s="14">
-        <v>17417</v>
+        <v>15000</v>
       </c>
       <c r="H25" s="15">
         <v>0</v>
@@ -2144,12 +2144,11 @@
         <v>11</v>
       </c>
       <c r="F26" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G26" s="14">
-        <f>17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H26" s="15">
         <v>0</v>
@@ -2172,12 +2171,11 @@
         <v>12</v>
       </c>
       <c r="F27" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G27" s="14">
-        <f t="shared" ref="G27:G31" si="0">17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H27" s="15">
         <v>0</v>
@@ -2200,11 +2198,10 @@
         <v>11</v>
       </c>
       <c r="F28" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G28" s="14">
-        <f t="shared" si="0"/>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H28" s="15">
         <v>0</v>
@@ -2227,11 +2224,10 @@
         <v>12</v>
       </c>
       <c r="F29" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G29" s="14">
-        <f t="shared" si="0"/>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H29" s="15">
         <v>0</v>
@@ -2254,12 +2250,11 @@
         <v>11</v>
       </c>
       <c r="F30" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G30" s="14">
-        <f t="shared" si="0"/>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H30" s="15">
         <v>0</v>
@@ -2282,12 +2277,11 @@
         <v>12</v>
       </c>
       <c r="F31" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G31" s="14">
-        <f t="shared" si="0"/>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H31" s="15">
         <v>0</v>
@@ -2310,11 +2304,10 @@
         <v>11</v>
       </c>
       <c r="F32" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G32" s="14">
-        <f>17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H32" s="15">
         <v>0</v>
@@ -2337,11 +2330,10 @@
         <v>12</v>
       </c>
       <c r="F33" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G33" s="14">
-        <f>17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H33" s="15">
         <v>0</v>
@@ -2364,11 +2356,10 @@
         <v>11</v>
       </c>
       <c r="F34" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G34" s="14">
-        <f>17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H34" s="15">
         <v>0</v>
@@ -2391,11 +2382,10 @@
         <v>12</v>
       </c>
       <c r="F35" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G35" s="14">
-        <f>17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H35" s="15">
         <v>0</v>
@@ -2418,11 +2408,10 @@
         <v>11</v>
       </c>
       <c r="F36" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G36" s="14">
-        <f t="shared" ref="G36:G37" si="1">17417+31519</f>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H36" s="15">
         <v>0</v>
@@ -2445,11 +2434,10 @@
         <v>12</v>
       </c>
       <c r="F37" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G37" s="14">
-        <f t="shared" si="1"/>
-        <v>48936</v>
+        <v>45000</v>
       </c>
       <c r="H37" s="15">
         <v>0</v>
@@ -2472,12 +2460,11 @@
         <v>11</v>
       </c>
       <c r="F38" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G38" s="14">
-        <f>17417+14818</f>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H38" s="15">
         <v>0</v>
@@ -2500,12 +2487,11 @@
         <v>12</v>
       </c>
       <c r="F39" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G39" s="14">
-        <f t="shared" ref="G39:G49" si="2">17417+14818</f>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H39" s="15">
         <v>0</v>
@@ -2528,11 +2514,10 @@
         <v>11</v>
       </c>
       <c r="F40" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G40" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H40" s="15">
         <v>0</v>
@@ -2555,11 +2540,10 @@
         <v>12</v>
       </c>
       <c r="F41" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G41" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H41" s="15">
         <v>0</v>
@@ -2582,12 +2566,11 @@
         <v>11</v>
       </c>
       <c r="F42" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G42" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H42" s="15">
         <v>0</v>
@@ -2610,12 +2593,11 @@
         <v>12</v>
       </c>
       <c r="F43" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G43" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H43" s="15">
         <v>0</v>
@@ -2638,11 +2620,10 @@
         <v>11</v>
       </c>
       <c r="F44" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G44" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H44" s="15">
         <v>0</v>
@@ -2665,11 +2646,10 @@
         <v>12</v>
       </c>
       <c r="F45" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G45" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H45" s="15">
         <v>0</v>
@@ -2692,11 +2672,10 @@
         <v>11</v>
       </c>
       <c r="F46" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G46" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H46" s="15">
         <v>0</v>
@@ -2719,11 +2698,10 @@
         <v>12</v>
       </c>
       <c r="F47" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G47" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H47" s="15">
         <v>0</v>
@@ -2746,11 +2724,10 @@
         <v>11</v>
       </c>
       <c r="F48" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G48" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H48" s="15">
         <v>0</v>
@@ -2773,11 +2750,10 @@
         <v>12</v>
       </c>
       <c r="F49" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G49" s="14">
-        <f t="shared" si="2"/>
-        <v>32235</v>
+        <v>30000</v>
       </c>
       <c r="H49" s="15">
         <v>0</v>
@@ -2800,11 +2776,11 @@
         <v>11</v>
       </c>
       <c r="F50" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G50" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H50" s="15">
         <v>0</v>
@@ -2827,11 +2803,11 @@
         <v>12</v>
       </c>
       <c r="F51" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G51" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H51" s="15">
         <v>0</v>
@@ -2854,10 +2830,10 @@
         <v>11</v>
       </c>
       <c r="F52" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G52" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H52" s="15">
         <v>0</v>
@@ -2880,10 +2856,10 @@
         <v>12</v>
       </c>
       <c r="F53" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G53" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H53" s="15">
         <v>0</v>
@@ -2906,11 +2882,11 @@
         <v>11</v>
       </c>
       <c r="F54" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G54" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H54" s="15">
         <v>0</v>
@@ -2933,11 +2909,11 @@
         <v>12</v>
       </c>
       <c r="F55" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G55" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H55" s="15">
         <v>0</v>
@@ -2960,10 +2936,10 @@
         <v>11</v>
       </c>
       <c r="F56" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G56" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H56" s="15">
         <v>0</v>
@@ -2986,10 +2962,10 @@
         <v>12</v>
       </c>
       <c r="F57" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G57" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H57" s="15">
         <v>0</v>
@@ -3012,10 +2988,10 @@
         <v>11</v>
       </c>
       <c r="F58" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G58" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H58" s="15">
         <v>0</v>
@@ -3038,10 +3014,10 @@
         <v>12</v>
       </c>
       <c r="F59" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G59" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H59" s="15">
         <v>0</v>
@@ -3064,10 +3040,10 @@
         <v>11</v>
       </c>
       <c r="F60" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G60" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H60" s="15">
         <v>0</v>
@@ -3090,10 +3066,10 @@
         <v>12</v>
       </c>
       <c r="F61" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G61" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H61" s="15">
         <v>0</v>
@@ -3116,11 +3092,11 @@
         <v>11</v>
       </c>
       <c r="F62" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G62" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H62" s="15">
         <v>0</v>
@@ -3143,11 +3119,11 @@
         <v>12</v>
       </c>
       <c r="F63" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G63" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H63" s="15">
         <v>0</v>
@@ -3170,10 +3146,10 @@
         <v>11</v>
       </c>
       <c r="F64" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G64" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H64" s="15">
         <v>0</v>
@@ -3196,10 +3172,10 @@
         <v>12</v>
       </c>
       <c r="F65" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G65" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H65" s="15">
         <v>0</v>
@@ -3222,11 +3198,11 @@
         <v>11</v>
       </c>
       <c r="F66" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G66" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H66" s="15">
         <v>0</v>
@@ -3249,11 +3225,11 @@
         <v>12</v>
       </c>
       <c r="F67" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G67" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H67" s="15">
         <v>0</v>
@@ -3276,10 +3252,10 @@
         <v>11</v>
       </c>
       <c r="F68" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G68" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H68" s="15">
         <v>0</v>
@@ -3302,10 +3278,10 @@
         <v>12</v>
       </c>
       <c r="F69" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G69" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H69" s="15">
         <v>0</v>
@@ -3328,10 +3304,10 @@
         <v>11</v>
       </c>
       <c r="F70" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G70" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H70" s="15">
         <v>0</v>
@@ -3354,10 +3330,10 @@
         <v>12</v>
       </c>
       <c r="F71" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G71" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H71" s="15">
         <v>0</v>
@@ -3380,10 +3356,10 @@
         <v>11</v>
       </c>
       <c r="F72" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G72" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H72" s="15">
         <v>0</v>
@@ -3406,10 +3382,10 @@
         <v>12</v>
       </c>
       <c r="F73" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G73" s="14">
-        <v>34833</v>
+        <v>35000</v>
       </c>
       <c r="H73" s="15">
         <v>0</v>
@@ -3432,12 +3408,11 @@
         <v>11</v>
       </c>
       <c r="F74" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G74" s="14">
-        <f>34833+30053</f>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H74" s="15">
         <v>0</v>
@@ -3460,12 +3435,11 @@
         <v>12</v>
       </c>
       <c r="F75" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G75" s="14">
-        <f t="shared" ref="G75:G85" si="3">34833+30053</f>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H75" s="15">
         <v>0</v>
@@ -3488,11 +3462,10 @@
         <v>11</v>
       </c>
       <c r="F76" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G76" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H76" s="15">
         <v>0</v>
@@ -3515,11 +3488,10 @@
         <v>12</v>
       </c>
       <c r="F77" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G77" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H77" s="15">
         <v>0</v>
@@ -3542,12 +3514,11 @@
         <v>11</v>
       </c>
       <c r="F78" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G78" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H78" s="15">
         <v>0</v>
@@ -3570,12 +3541,11 @@
         <v>12</v>
       </c>
       <c r="F79" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G79" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H79" s="15">
         <v>0</v>
@@ -3598,11 +3568,10 @@
         <v>11</v>
       </c>
       <c r="F80" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G80" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H80" s="15">
         <v>0</v>
@@ -3625,11 +3594,10 @@
         <v>12</v>
       </c>
       <c r="F81" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G81" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H81" s="15">
         <v>0</v>
@@ -3652,11 +3620,10 @@
         <v>11</v>
       </c>
       <c r="F82" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G82" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H82" s="15">
         <v>0</v>
@@ -3679,11 +3646,10 @@
         <v>12</v>
       </c>
       <c r="F83" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G83" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H83" s="15">
         <v>0</v>
@@ -3706,11 +3672,10 @@
         <v>11</v>
       </c>
       <c r="F84" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G84" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H84" s="15">
         <v>0</v>
@@ -3733,11 +3698,10 @@
         <v>12</v>
       </c>
       <c r="F85" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G85" s="14">
-        <f t="shared" si="3"/>
-        <v>64886</v>
+        <v>65000</v>
       </c>
       <c r="H85" s="15">
         <v>0</v>
@@ -3760,12 +3724,11 @@
         <v>11</v>
       </c>
       <c r="F86" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G86" s="14">
-        <f>34833+14101</f>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H86" s="15">
         <v>0</v>
@@ -3788,12 +3751,11 @@
         <v>12</v>
       </c>
       <c r="F87" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G87" s="14">
-        <f t="shared" ref="G87:G97" si="4">34833+14101</f>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H87" s="15">
         <v>0</v>
@@ -3816,11 +3778,10 @@
         <v>11</v>
       </c>
       <c r="F88" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G88" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H88" s="15">
         <v>0</v>
@@ -3843,11 +3804,10 @@
         <v>12</v>
       </c>
       <c r="F89" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G89" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H89" s="15">
         <v>0</v>
@@ -3870,12 +3830,11 @@
         <v>11</v>
       </c>
       <c r="F90" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G90" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H90" s="15">
         <v>0</v>
@@ -3898,12 +3857,11 @@
         <v>12</v>
       </c>
       <c r="F91" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G91" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H91" s="15">
         <v>0</v>
@@ -3926,11 +3884,10 @@
         <v>11</v>
       </c>
       <c r="F92" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G92" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H92" s="15">
         <v>0</v>
@@ -3953,11 +3910,10 @@
         <v>12</v>
       </c>
       <c r="F93" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G93" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H93" s="15">
         <v>0</v>
@@ -3980,11 +3936,10 @@
         <v>11</v>
       </c>
       <c r="F94" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G94" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H94" s="15">
         <v>0</v>
@@ -4007,11 +3962,10 @@
         <v>12</v>
       </c>
       <c r="F95" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G95" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H95" s="15">
         <v>0</v>
@@ -4034,11 +3988,10 @@
         <v>11</v>
       </c>
       <c r="F96" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G96" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H96" s="15">
         <v>0</v>
@@ -4061,11 +4014,10 @@
         <v>12</v>
       </c>
       <c r="F97" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G97" s="14">
-        <f t="shared" si="4"/>
-        <v>48934</v>
+        <v>50000</v>
       </c>
       <c r="H97" s="15">
         <v>0</v>
@@ -4088,11 +4040,11 @@
         <v>11</v>
       </c>
       <c r="F98" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G98" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H98" s="15">
         <v>0</v>
@@ -4115,11 +4067,11 @@
         <v>12</v>
       </c>
       <c r="F99" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G99" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H99" s="15">
         <v>0</v>
@@ -4142,10 +4094,10 @@
         <v>11</v>
       </c>
       <c r="F100" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G100" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H100" s="15">
         <v>0</v>
@@ -4168,10 +4120,10 @@
         <v>12</v>
       </c>
       <c r="F101" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G101" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H101" s="15">
         <v>0</v>
@@ -4194,11 +4146,11 @@
         <v>11</v>
       </c>
       <c r="F102" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G102" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H102" s="15">
         <v>0</v>
@@ -4221,11 +4173,11 @@
         <v>12</v>
       </c>
       <c r="F103" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G103" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H103" s="15">
         <v>0</v>
@@ -4248,10 +4200,10 @@
         <v>11</v>
       </c>
       <c r="F104" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G104" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H104" s="15">
         <v>0</v>
@@ -4274,10 +4226,10 @@
         <v>12</v>
       </c>
       <c r="F105" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G105" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H105" s="15">
         <v>0</v>
@@ -4300,10 +4252,10 @@
         <v>11</v>
       </c>
       <c r="F106" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G106" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H106" s="15">
         <v>0</v>
@@ -4326,10 +4278,10 @@
         <v>12</v>
       </c>
       <c r="F107" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G107" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H107" s="15">
         <v>0</v>
@@ -4352,10 +4304,10 @@
         <v>11</v>
       </c>
       <c r="F108" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G108" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H108" s="15">
         <v>0</v>
@@ -4378,10 +4330,10 @@
         <v>12</v>
       </c>
       <c r="F109" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G109" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H109" s="15">
         <v>0</v>
@@ -4404,11 +4356,11 @@
         <v>11</v>
       </c>
       <c r="F110" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G110" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H110" s="15">
         <v>0</v>
@@ -4431,11 +4383,11 @@
         <v>12</v>
       </c>
       <c r="F111" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G111" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H111" s="15">
         <v>0</v>
@@ -4458,10 +4410,10 @@
         <v>11</v>
       </c>
       <c r="F112" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G112" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H112" s="15">
         <v>0</v>
@@ -4484,10 +4436,10 @@
         <v>12</v>
       </c>
       <c r="F113" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G113" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H113" s="15">
         <v>0</v>
@@ -4510,11 +4462,11 @@
         <v>11</v>
       </c>
       <c r="F114" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G114" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H114" s="15">
         <v>0</v>
@@ -4537,11 +4489,11 @@
         <v>12</v>
       </c>
       <c r="F115" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G115" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H115" s="15">
         <v>0</v>
@@ -4564,10 +4516,10 @@
         <v>11</v>
       </c>
       <c r="F116" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G116" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H116" s="15">
         <v>0</v>
@@ -4590,10 +4542,10 @@
         <v>12</v>
       </c>
       <c r="F117" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G117" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H117" s="15">
         <v>0</v>
@@ -4616,10 +4568,10 @@
         <v>11</v>
       </c>
       <c r="F118" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G118" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H118" s="15">
         <v>0</v>
@@ -4642,10 +4594,10 @@
         <v>12</v>
       </c>
       <c r="F119" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G119" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H119" s="15">
         <v>0</v>
@@ -4668,10 +4620,10 @@
         <v>11</v>
       </c>
       <c r="F120" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G120" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H120" s="15">
         <v>0</v>
@@ -4694,10 +4646,10 @@
         <v>12</v>
       </c>
       <c r="F121" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G121" s="14">
-        <v>52250</v>
+        <v>55000</v>
       </c>
       <c r="H121" s="15">
         <v>0</v>
@@ -4720,12 +4672,11 @@
         <v>11</v>
       </c>
       <c r="F122" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G122" s="14">
-        <f>52250+28587</f>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H122" s="15">
         <v>0</v>
@@ -4748,12 +4699,11 @@
         <v>12</v>
       </c>
       <c r="F123" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G123" s="14">
-        <f t="shared" ref="G123:G133" si="5">52250+28587</f>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H123" s="15">
         <v>0</v>
@@ -4776,11 +4726,10 @@
         <v>11</v>
       </c>
       <c r="F124" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G124" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H124" s="15">
         <v>0</v>
@@ -4803,11 +4752,10 @@
         <v>12</v>
       </c>
       <c r="F125" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G125" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H125" s="15">
         <v>0</v>
@@ -4830,12 +4778,11 @@
         <v>11</v>
       </c>
       <c r="F126" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G126" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H126" s="15">
         <v>0</v>
@@ -4858,12 +4805,11 @@
         <v>12</v>
       </c>
       <c r="F127" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G127" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H127" s="15">
         <v>0</v>
@@ -4886,11 +4832,10 @@
         <v>11</v>
       </c>
       <c r="F128" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G128" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H128" s="15">
         <v>0</v>
@@ -4913,11 +4858,10 @@
         <v>12</v>
       </c>
       <c r="F129" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G129" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H129" s="15">
         <v>0</v>
@@ -4940,11 +4884,10 @@
         <v>11</v>
       </c>
       <c r="F130" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G130" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H130" s="15">
         <v>0</v>
@@ -4967,11 +4910,10 @@
         <v>12</v>
       </c>
       <c r="F131" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G131" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H131" s="15">
         <v>0</v>
@@ -4994,11 +4936,10 @@
         <v>11</v>
       </c>
       <c r="F132" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G132" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H132" s="15">
         <v>0</v>
@@ -5021,11 +4962,10 @@
         <v>12</v>
       </c>
       <c r="F133" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G133" s="14">
-        <f t="shared" si="5"/>
-        <v>80837</v>
+        <v>85000</v>
       </c>
       <c r="H133" s="15">
         <v>0</v>
@@ -5048,12 +4988,11 @@
         <v>11</v>
       </c>
       <c r="F134" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G134" s="14">
-        <f>52250+13384</f>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H134" s="15">
         <v>0</v>
@@ -5076,12 +5015,11 @@
         <v>12</v>
       </c>
       <c r="F135" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G135" s="14">
-        <f t="shared" ref="G135:G145" si="6">52250+13384</f>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H135" s="15">
         <v>0</v>
@@ -5104,11 +5042,10 @@
         <v>11</v>
       </c>
       <c r="F136" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G136" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H136" s="15">
         <v>0</v>
@@ -5131,11 +5068,10 @@
         <v>12</v>
       </c>
       <c r="F137" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G137" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H137" s="15">
         <v>0</v>
@@ -5158,12 +5094,11 @@
         <v>11</v>
       </c>
       <c r="F138" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G138" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H138" s="15">
         <v>0</v>
@@ -5186,12 +5121,11 @@
         <v>12</v>
       </c>
       <c r="F139" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G139" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H139" s="15">
         <v>0</v>
@@ -5214,11 +5148,10 @@
         <v>11</v>
       </c>
       <c r="F140" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G140" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H140" s="15">
         <v>0</v>
@@ -5241,11 +5174,10 @@
         <v>12</v>
       </c>
       <c r="F141" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G141" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H141" s="15">
         <v>0</v>
@@ -5268,11 +5200,10 @@
         <v>11</v>
       </c>
       <c r="F142" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G142" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H142" s="15">
         <v>0</v>
@@ -5295,11 +5226,10 @@
         <v>12</v>
       </c>
       <c r="F143" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G143" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H143" s="15">
         <v>0</v>
@@ -5322,11 +5252,10 @@
         <v>11</v>
       </c>
       <c r="F144" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G144" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H144" s="15">
         <v>0</v>
@@ -5349,11 +5278,10 @@
         <v>12</v>
       </c>
       <c r="F145" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G145" s="14">
-        <f t="shared" si="6"/>
-        <v>65634</v>
+        <v>70000</v>
       </c>
       <c r="H145" s="15">
         <v>0</v>
@@ -5376,11 +5304,11 @@
         <v>11</v>
       </c>
       <c r="F146" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G146" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H146" s="15">
         <v>0</v>
@@ -5403,11 +5331,11 @@
         <v>12</v>
       </c>
       <c r="F147" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G147" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H147" s="15">
         <v>0</v>
@@ -5430,10 +5358,10 @@
         <v>11</v>
       </c>
       <c r="F148" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G148" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H148" s="15">
         <v>0</v>
@@ -5456,10 +5384,10 @@
         <v>12</v>
       </c>
       <c r="F149" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G149" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H149" s="15">
         <v>0</v>
@@ -5482,11 +5410,11 @@
         <v>11</v>
       </c>
       <c r="F150" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G150" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H150" s="15">
         <v>0</v>
@@ -5509,11 +5437,11 @@
         <v>12</v>
       </c>
       <c r="F151" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G151" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H151" s="15">
         <v>0</v>
@@ -5536,10 +5464,10 @@
         <v>11</v>
       </c>
       <c r="F152" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G152" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H152" s="15">
         <v>0</v>
@@ -5562,10 +5490,10 @@
         <v>12</v>
       </c>
       <c r="F153" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G153" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H153" s="15">
         <v>0</v>
@@ -5588,10 +5516,10 @@
         <v>11</v>
       </c>
       <c r="F154" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G154" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H154" s="15">
         <v>0</v>
@@ -5614,10 +5542,10 @@
         <v>12</v>
       </c>
       <c r="F155" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G155" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H155" s="15">
         <v>0</v>
@@ -5640,10 +5568,10 @@
         <v>11</v>
       </c>
       <c r="F156" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G156" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H156" s="15">
         <v>0</v>
@@ -5666,10 +5594,10 @@
         <v>12</v>
       </c>
       <c r="F157" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G157" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H157" s="15">
         <v>0</v>
@@ -5692,11 +5620,11 @@
         <v>11</v>
       </c>
       <c r="F158" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G158" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H158" s="15">
         <v>0</v>
@@ -5719,11 +5647,11 @@
         <v>12</v>
       </c>
       <c r="F159" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G159" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H159" s="15">
         <v>0</v>
@@ -5746,10 +5674,10 @@
         <v>11</v>
       </c>
       <c r="F160" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G160" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H160" s="15">
         <v>0</v>
@@ -5772,10 +5700,10 @@
         <v>12</v>
       </c>
       <c r="F161" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G161" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H161" s="15">
         <v>0</v>
@@ -5798,11 +5726,11 @@
         <v>11</v>
       </c>
       <c r="F162" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G162" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H162" s="15">
         <v>0</v>
@@ -5825,11 +5753,11 @@
         <v>12</v>
       </c>
       <c r="F163" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G163" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H163" s="15">
         <v>0</v>
@@ -5852,10 +5780,10 @@
         <v>11</v>
       </c>
       <c r="F164" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G164" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H164" s="15">
         <v>0</v>
@@ -5878,10 +5806,10 @@
         <v>12</v>
       </c>
       <c r="F165" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G165" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H165" s="15">
         <v>0</v>
@@ -5904,10 +5832,10 @@
         <v>11</v>
       </c>
       <c r="F166" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G166" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H166" s="15">
         <v>0</v>
@@ -5930,10 +5858,10 @@
         <v>12</v>
       </c>
       <c r="F167" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G167" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H167" s="15">
         <v>0</v>
@@ -5956,10 +5884,10 @@
         <v>11</v>
       </c>
       <c r="F168" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G168" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H168" s="15">
         <v>0</v>
@@ -5982,10 +5910,10 @@
         <v>12</v>
       </c>
       <c r="F169" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G169" s="14">
-        <v>69677</v>
+        <v>65000</v>
       </c>
       <c r="H169" s="15">
         <v>0</v>
@@ -6008,12 +5936,11 @@
         <v>11</v>
       </c>
       <c r="F170" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G170" s="14">
-        <f>69677+27121</f>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H170" s="15">
         <v>0</v>
@@ -6036,12 +5963,11 @@
         <v>12</v>
       </c>
       <c r="F171" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G171" s="14">
-        <f t="shared" ref="G171:G181" si="7">69677+27121</f>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H171" s="15">
         <v>0</v>
@@ -6064,11 +5990,10 @@
         <v>11</v>
       </c>
       <c r="F172" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G172" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H172" s="15">
         <v>0</v>
@@ -6091,11 +6016,10 @@
         <v>12</v>
       </c>
       <c r="F173" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G173" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H173" s="15">
         <v>0</v>
@@ -6118,12 +6042,11 @@
         <v>11</v>
       </c>
       <c r="F174" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G174" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H174" s="15">
         <v>0</v>
@@ -6146,12 +6069,11 @@
         <v>12</v>
       </c>
       <c r="F175" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G175" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H175" s="15">
         <v>0</v>
@@ -6174,11 +6096,10 @@
         <v>11</v>
       </c>
       <c r="F176" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G176" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H176" s="15">
         <v>0</v>
@@ -6201,11 +6122,10 @@
         <v>12</v>
       </c>
       <c r="F177" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G177" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H177" s="15">
         <v>0</v>
@@ -6228,11 +6148,10 @@
         <v>11</v>
       </c>
       <c r="F178" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G178" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H178" s="15">
         <v>0</v>
@@ -6255,11 +6174,10 @@
         <v>12</v>
       </c>
       <c r="F179" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G179" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H179" s="15">
         <v>0</v>
@@ -6282,11 +6200,10 @@
         <v>11</v>
       </c>
       <c r="F180" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G180" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H180" s="15">
         <v>0</v>
@@ -6309,11 +6226,10 @@
         <v>12</v>
       </c>
       <c r="F181" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G181" s="14">
-        <f t="shared" si="7"/>
-        <v>96798</v>
+        <v>90000</v>
       </c>
       <c r="H181" s="15">
         <v>0</v>
@@ -6336,12 +6252,11 @@
         <v>11</v>
       </c>
       <c r="F182" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G182" s="14">
-        <f>69677+12667</f>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H182" s="15">
         <v>0</v>
@@ -6364,12 +6279,11 @@
         <v>12</v>
       </c>
       <c r="F183" s="13">
-        <f>309598</f>
-        <v>309598</v>
+        <f>295000</f>
+        <v>295000</v>
       </c>
       <c r="G183" s="14">
-        <f t="shared" ref="G183:G186" si="8">69677+12667</f>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H183" s="15">
         <v>0</v>
@@ -6392,11 +6306,10 @@
         <v>11</v>
       </c>
       <c r="F184" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G184" s="14">
-        <f t="shared" si="8"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H184" s="15">
         <v>0</v>
@@ -6419,11 +6332,10 @@
         <v>12</v>
       </c>
       <c r="F185" s="13">
-        <v>154799</v>
+        <v>150000</v>
       </c>
       <c r="G185" s="14">
-        <f t="shared" si="8"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H185" s="15">
         <v>0</v>
@@ -6446,12 +6358,11 @@
         <v>11</v>
       </c>
       <c r="F186" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G186" s="14">
-        <f t="shared" si="8"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H186" s="15">
         <v>0</v>
@@ -6474,12 +6385,11 @@
         <v>12</v>
       </c>
       <c r="F187" s="13">
-        <f>3616</f>
-        <v>3616</v>
+        <f>3000</f>
+        <v>3000</v>
       </c>
       <c r="G187" s="14">
-        <f>69677+12667</f>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H187" s="15">
         <v>0</v>
@@ -6502,11 +6412,10 @@
         <v>11</v>
       </c>
       <c r="F188" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G188" s="14">
-        <f t="shared" ref="G188:G193" si="9">69677+12667</f>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H188" s="15">
         <v>0</v>
@@ -6529,11 +6438,10 @@
         <v>12</v>
       </c>
       <c r="F189" s="13">
-        <v>219311</v>
+        <v>210000</v>
       </c>
       <c r="G189" s="14">
-        <f t="shared" si="9"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H189" s="15">
         <v>0</v>
@@ -6556,11 +6464,10 @@
         <v>11</v>
       </c>
       <c r="F190" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G190" s="14">
-        <f t="shared" si="9"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H190" s="15">
         <v>0</v>
@@ -6583,11 +6490,10 @@
         <v>12</v>
       </c>
       <c r="F191" s="13">
-        <v>26551</v>
+        <v>25000</v>
       </c>
       <c r="G191" s="14">
-        <f t="shared" si="9"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H191" s="15">
         <v>0</v>
@@ -6610,11 +6516,10 @@
         <v>11</v>
       </c>
       <c r="F192" s="13">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G192" s="14">
-        <f t="shared" si="9"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H192" s="15">
         <v>0</v>
@@ -6637,11 +6542,10 @@
         <v>12</v>
       </c>
       <c r="F193" s="19">
-        <v>2595</v>
+        <v>2500</v>
       </c>
       <c r="G193" s="20">
-        <f t="shared" si="9"/>
-        <v>82344</v>
+        <v>75000</v>
       </c>
       <c r="H193" s="21">
         <v>0</v>
@@ -6658,7 +6562,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6703,31 +6607,31 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="B2" s="59">
-        <v>4.37</v>
+        <v>4.25</v>
       </c>
       <c r="C2" s="59">
-        <v>1.9</v>
+        <v>1.75</v>
       </c>
       <c r="D2" s="60">
-        <v>282300000</v>
+        <v>275000000</v>
       </c>
       <c r="E2" s="61">
-        <v>100400000</v>
+        <v>100000000</v>
       </c>
       <c r="F2" s="59">
-        <v>5.27</v>
+        <v>5.15</v>
       </c>
       <c r="G2" s="59">
-        <v>3.84</v>
+        <v>3.75</v>
       </c>
       <c r="H2" s="62">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="I2" s="63">
-        <v>1</v>
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>
@@ -6741,7 +6645,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6793,7 +6697,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="47">
-        <v>0.19949999999999998</v>
+        <v>0.19750000000000001</v>
       </c>
       <c r="C2" s="47">
         <v>0</v>
@@ -6802,28 +6706,28 @@
         <v>0</v>
       </c>
       <c r="E2" s="47">
-        <v>0.22799999999999998</v>
+        <v>0.249</v>
       </c>
       <c r="F2" s="47">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="G2" s="53">
-        <v>0.95000000000000007</v>
+        <v>0.9</v>
       </c>
       <c r="H2" s="53">
-        <v>1.8136363636363633</v>
+        <v>1.7136363636363601</v>
       </c>
       <c r="I2" s="53">
-        <v>1.1083333333333332</v>
+        <v>1.30833333333333</v>
       </c>
       <c r="J2" s="53">
-        <v>0.58676470588235285</v>
+        <v>0.78676470588235303</v>
       </c>
       <c r="K2" s="53">
-        <v>0.43369565217391298</v>
+        <v>0.53369565217391302</v>
       </c>
       <c r="L2" s="48">
-        <v>0.62343749999999998</v>
+        <v>0.72343749999999996</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6831,7 +6735,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="47">
-        <v>0.189</v>
+        <v>0.185</v>
       </c>
       <c r="C3" s="47">
         <v>0</v>
@@ -6840,28 +6744,28 @@
         <v>0</v>
       </c>
       <c r="E3" s="47">
-        <v>0.216</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="F3" s="47">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="G3" s="53">
-        <v>0.89999999999999991</v>
+        <v>0.85</v>
       </c>
       <c r="H3" s="53">
-        <v>1.7181818181818183</v>
+        <v>1.6181818181818199</v>
       </c>
       <c r="I3" s="53">
-        <v>1.05</v>
+        <v>1.25</v>
       </c>
       <c r="J3" s="53">
-        <v>0.55588235294117638</v>
+        <v>0.65588235294117603</v>
       </c>
       <c r="K3" s="53">
-        <v>0.41086956521739126</v>
+        <v>0.46086956521739098</v>
       </c>
       <c r="L3" s="48">
-        <v>0.59062499999999996</v>
+        <v>0.69062500000000004</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6869,7 +6773,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="47">
-        <v>0.17849999999999999</v>
+        <v>0.17249999999999999</v>
       </c>
       <c r="C4" s="47">
         <v>0</v>
@@ -6878,28 +6782,28 @@
         <v>0</v>
       </c>
       <c r="E4" s="47">
-        <v>0.20399999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="F4" s="47">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G4" s="53">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="H4" s="53">
-        <v>1.6227272727272726</v>
+        <v>1.52272727272727</v>
       </c>
       <c r="I4" s="53">
-        <v>0.9916666666666667</v>
+        <v>0.89166666666666705</v>
       </c>
       <c r="J4" s="53">
-        <v>0.52500000000000002</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="K4" s="53">
-        <v>0.38804347826086955</v>
+        <v>0.33804347826087</v>
       </c>
       <c r="L4" s="48">
-        <v>0.55781249999999993</v>
+        <v>0.45781250000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -6907,7 +6811,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="49">
-        <v>0.16800000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="C5" s="49">
         <v>0</v>
@@ -6916,28 +6820,28 @@
         <v>0</v>
       </c>
       <c r="E5" s="49">
-        <v>0.192</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="F5" s="49">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="G5" s="50">
-        <v>0.80000000000000016</v>
+        <v>0.7</v>
       </c>
       <c r="H5" s="50">
-        <v>1.5272727272727273</v>
+        <v>1.4272727272727299</v>
       </c>
       <c r="I5" s="50">
-        <v>0.93333333333333335</v>
+        <v>0.73333333333333295</v>
       </c>
       <c r="J5" s="50">
-        <v>0.49411764705882355</v>
+        <v>0.39411764705882402</v>
       </c>
       <c r="K5" s="50">
-        <v>0.36521739130434783</v>
+        <v>0.26521739130434802</v>
       </c>
       <c r="L5" s="51">
-        <v>0.52500000000000002</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -6950,8 +6854,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6986,10 +6890,10 @@
         <v>34</v>
       </c>
       <c r="C2" s="33">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D2" s="34">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>35</v>
@@ -7033,10 +6937,10 @@
         <v>34</v>
       </c>
       <c r="C5" s="37">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D5" s="38">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>35</v>
@@ -7050,10 +6954,10 @@
         <v>38</v>
       </c>
       <c r="C6" s="37">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D6" s="38">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>35</v>
@@ -7082,10 +6986,10 @@
         <v>40</v>
       </c>
       <c r="C8" s="33">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D8" s="34">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>41</v>
@@ -7099,10 +7003,10 @@
         <v>40</v>
       </c>
       <c r="C9" s="42">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="43">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>41</v>

</xml_diff>